<commit_message>
fix- shift manager cant put Constrains before all workers and worker cant put if he already put
</commit_message>
<xml_diff>
--- a/final project/presence1.xlsx
+++ b/final project/presence1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>index</t>
   </si>
@@ -55,7 +55,7 @@
     <t>12</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 20:08:16</t>
+    <t>Fri, 04 Jan 2019 11:07:04</t>
   </si>
   <si>
     <t>asaf</t>
@@ -79,15 +79,12 @@
     <t>Sun, 16 Dec 2018 11:08:16</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 21:31:09</t>
+    <t>Fri, 04 Jan 2019 10:44:37</t>
   </si>
   <si>
     <t>Sun, 16 Dec 2018 21:08:16</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 21:27:02</t>
-  </si>
-  <si>
     <t>emilia</t>
   </si>
   <si>
@@ -142,13 +139,13 @@
     <t>Wed, 02 Jan 2019 11:17:29</t>
   </si>
   <si>
-    <t>Thu, 03 Jan 2019 16:08:20</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>Fri, 04 Jan 2019 11:03:40</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Fri, 04 Jan 2019 11:07:17</t>
   </si>
 </sst>
 </file>
@@ -480,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="I4">
-        <v>37373</v>
+        <v>-1419</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -625,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I5">
         <v>1126</v>
@@ -636,13 +633,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -654,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>112</v>
@@ -665,25 +662,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
       </c>
       <c r="I7">
         <v>21</v>
@@ -697,22 +694,22 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>37</v>
       </c>
       <c r="I8">
         <v>119</v>
@@ -723,25 +720,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
       </c>
       <c r="I9">
         <v>107</v>
@@ -752,22 +749,51 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>